<commit_message>
changes from re-running notebooks, order different
</commit_message>
<xml_diff>
--- a/nlp/gen_goods.xlsx
+++ b/nlp/gen_goods.xlsx
@@ -58,24 +58,24 @@
     <t>гарусный товар</t>
   </si>
   <si>
+    <t>особливый товар</t>
+  </si>
+  <si>
     <t>мелочь</t>
   </si>
   <si>
-    <t>особливый товар</t>
-  </si>
-  <si>
     <t>серебреный товар</t>
   </si>
   <si>
     <t>деревенский товар</t>
   </si>
   <si>
+    <t>небогатый товар</t>
+  </si>
+  <si>
     <t>крамными товар</t>
   </si>
   <si>
-    <t>небогатый товар</t>
-  </si>
-  <si>
     <t>мясо</t>
   </si>
   <si>
@@ -88,61 +88,61 @@
     <t>щепетильный товар</t>
   </si>
   <si>
+    <t>пушной товар</t>
+  </si>
+  <si>
     <t>нужный товар</t>
   </si>
   <si>
-    <t>пушной товар</t>
-  </si>
-  <si>
     <t>набойчатый товар</t>
   </si>
   <si>
+    <t>суровский товар</t>
+  </si>
+  <si>
     <t>недорогой товар</t>
   </si>
   <si>
     <t>медный товар</t>
   </si>
   <si>
-    <t>суровский товар</t>
+    <t>внутренний товар</t>
   </si>
   <si>
     <t>питейный припасы</t>
   </si>
   <si>
-    <t>внутренний товар</t>
-  </si>
-  <si>
     <t>привозный товар</t>
   </si>
   <si>
     <t>оловянный товар</t>
   </si>
   <si>
+    <t>заморский товар</t>
+  </si>
+  <si>
+    <t>купецкий товар</t>
+  </si>
+  <si>
     <t>произрастание</t>
   </si>
   <si>
-    <t>заморский товар</t>
-  </si>
-  <si>
     <t>галантерейный товар</t>
   </si>
   <si>
-    <t>купецкий товар</t>
+    <t>рукодельный товар</t>
+  </si>
+  <si>
+    <t>меховой товар</t>
+  </si>
+  <si>
+    <t>домовый товар</t>
   </si>
   <si>
     <t>надлежащий товар</t>
   </si>
   <si>
-    <t>домовый товар</t>
-  </si>
-  <si>
     <t>харчевой припасы</t>
-  </si>
-  <si>
-    <t>рукодельный товар</t>
-  </si>
-  <si>
-    <t>меховой товар</t>
   </si>
 </sst>
 </file>

</xml_diff>